<commit_message>
Ajout 1ère partie Gui
Integration d'une interface graphique avec :
+ Choix projet
+ Horizon
+Durée investissements
+ Choix Activités
+ Plan d'investissement
+ Plan de Financement
</commit_message>
<xml_diff>
--- a/module classe projet/ModulePrincipal/CPC.xlsx
+++ b/module classe projet/ModulePrincipal/CPC.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>Couts</t>
   </si>
@@ -34,19 +34,22 @@
     <t>t = 5</t>
   </si>
   <si>
-    <t>Prestation de soins médicaux</t>
+    <t xml:space="preserve">Prestation de cours </t>
+  </si>
+  <si>
+    <t>Couts d'assurance</t>
+  </si>
+  <si>
+    <t>Cout de location, espace</t>
+  </si>
+  <si>
+    <t>Cout d'energie, électricité</t>
+  </si>
+  <si>
+    <t>Total des couts</t>
   </si>
   <si>
     <t>Cout d'entretien</t>
-  </si>
-  <si>
-    <t>Cout RH</t>
-  </si>
-  <si>
-    <t>Cout des consommables de santé</t>
-  </si>
-  <si>
-    <t>Total des couts</t>
   </si>
 </sst>
 </file>
@@ -360,7 +363,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K13" sqref="A1:K13"/>
@@ -407,19 +410,19 @@
         <v>7</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -427,19 +430,19 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -447,25 +450,28 @@
         <v>9</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>10</v>
       </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
@@ -480,6 +486,106 @@
       </c>
       <c r="G6" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="n">
+        <v>75</v>
+      </c>
+      <c r="D8" t="n">
+        <v>75</v>
+      </c>
+      <c r="E8" t="n">
+        <v>75</v>
+      </c>
+      <c r="F8" t="n">
+        <v>75</v>
+      </c>
+      <c r="G8" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="n">
+        <v>84</v>
+      </c>
+      <c r="D9" t="n">
+        <v>84</v>
+      </c>
+      <c r="E9" t="n">
+        <v>84</v>
+      </c>
+      <c r="F9" t="n">
+        <v>84</v>
+      </c>
+      <c r="G9" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="n">
+        <v>322</v>
+      </c>
+      <c r="D11" t="n">
+        <v>322</v>
+      </c>
+      <c r="E11" t="n">
+        <v>322</v>
+      </c>
+      <c r="F11" t="n">
+        <v>322</v>
+      </c>
+      <c r="G11" t="n">
+        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>